<commit_message>
added updated_by colom in db and also according to it fixed backend files excel,editstudent,fileupload, added new db, added middle wear in upload file routes
</commit_message>
<xml_diff>
--- a/Frontend/public/templates/placement_template.xlsx
+++ b/Frontend/public/templates/placement_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\UGSF\UGSF_TNP\Frontend\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -46,9 +46,6 @@
     <t>position</t>
   </si>
   <si>
-    <t>package</t>
-  </si>
-  <si>
     <t>university_name</t>
   </si>
   <si>
@@ -767,6 +764,9 @@
   </si>
   <si>
     <t>22DCE059</t>
+  </si>
+  <si>
+    <t>salary_package</t>
   </si>
 </sst>
 </file>
@@ -1286,17 +1286,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
@@ -1304,47 +1304,47 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
@@ -1352,7 +1352,7 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
@@ -1360,37 +1360,37 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
@@ -1398,117 +1398,117 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" s="19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
@@ -1516,47 +1516,47 @@
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.3">
@@ -1564,7 +1564,7 @@
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.3">
@@ -1572,82 +1572,82 @@
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" s="19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.3">
@@ -1658,7 +1658,7 @@
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.3">
@@ -1666,222 +1666,222 @@
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A95" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104" s="17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106" s="17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107" s="17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109" s="17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A119" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A123" s="21" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A124" s="21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A125" s="21" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A126" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A127" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A128" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A129" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A130" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A131" s="21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A132" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A133" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A134" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A136" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1900,8 +1900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q844"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1926,7 +1926,7 @@
   <sheetData>
     <row r="1" spans="1:17" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>
@@ -1938,7 +1938,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F1" s="10" t="s">
         <v>3</v>
@@ -1956,36 +1956,36 @@
         <v>7</v>
       </c>
       <c r="K1" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="N1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="10" t="s">
         <v>14</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="P1" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="10" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>131</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>132</v>
       </c>
       <c r="D2" s="8">
         <v>2022</v>
@@ -1994,25 +1994,25 @@
         <v>2022</v>
       </c>
       <c r="F2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>17</v>
-      </c>
       <c r="I2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>21</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>22</v>
       </c>
       <c r="K2" s="8">
         <v>2500000</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>

</xml_diff>